<commit_message>
refactor(capacity_report): update comparison column names and calculations
- Replace static column names with dynamic ones using date variables
- Simplify change calculations by referencing computed column names
- Remove commented-out column width configuration lines
</commit_message>
<xml_diff>
--- a/02-Feb-26.xlsx
+++ b/02-Feb-26.xlsx
@@ -2790,27 +2790,27 @@
       </c>
       <c r="M53" s="6" t="inlineStr">
         <is>
-          <t>Yesterday Qty. (Mar)</t>
+          <t>02-Feb (Mar)</t>
         </is>
       </c>
       <c r="N53" s="6" t="inlineStr">
         <is>
-          <t>Today Qty. (Mar)</t>
+          <t>01-Feb (Mar)</t>
         </is>
       </c>
       <c r="O53" s="6" t="inlineStr">
         <is>
-          <t>Yesterday Qty. (Apr)</t>
+          <t>Change (Mar)</t>
         </is>
       </c>
       <c r="P53" s="6" t="inlineStr">
         <is>
-          <t>Today Qty. (Apr)</t>
+          <t>02-Feb (Apr)</t>
         </is>
       </c>
       <c r="Q53" s="6" t="inlineStr">
         <is>
-          <t>Change (Mar)</t>
+          <t>01-Feb (Apr)</t>
         </is>
       </c>
       <c r="R53" s="6" t="inlineStr">
@@ -2833,19 +2833,19 @@
         </is>
       </c>
       <c r="M54" s="8" t="n">
+        <v>1219155</v>
+      </c>
+      <c r="N54" s="8" t="n">
         <v>850580</v>
       </c>
-      <c r="N54" s="8" t="n">
-        <v>1219155</v>
-      </c>
       <c r="O54" s="8" t="n">
-        <v>143975</v>
+        <v>368575</v>
       </c>
       <c r="P54" s="8" t="n">
         <v>248119</v>
       </c>
       <c r="Q54" s="8" t="n">
-        <v>368575</v>
+        <v>143975</v>
       </c>
       <c r="R54" s="8" t="n">
         <v>104144</v>
@@ -2865,19 +2865,19 @@
         </is>
       </c>
       <c r="M55" s="8" t="n">
+        <v>833429</v>
+      </c>
+      <c r="N55" s="8" t="n">
         <v>832571</v>
       </c>
-      <c r="N55" s="8" t="n">
-        <v>833429</v>
-      </c>
       <c r="O55" s="8" t="n">
-        <v>6462</v>
+        <v>858</v>
       </c>
       <c r="P55" s="8" t="n">
         <v>6462</v>
       </c>
       <c r="Q55" s="8" t="n">
-        <v>858</v>
+        <v>6462</v>
       </c>
       <c r="R55" s="8" t="n">
         <v>0</v>
@@ -2890,19 +2890,19 @@
         </is>
       </c>
       <c r="M56" s="8" t="n">
+        <v>998102</v>
+      </c>
+      <c r="N56" s="8" t="n">
         <v>989030</v>
       </c>
-      <c r="N56" s="8" t="n">
-        <v>998102</v>
-      </c>
       <c r="O56" s="8" t="n">
-        <v>959279</v>
+        <v>9072</v>
       </c>
       <c r="P56" s="8" t="n">
         <v>959287</v>
       </c>
       <c r="Q56" s="8" t="n">
-        <v>9072</v>
+        <v>959279</v>
       </c>
       <c r="R56" s="8" t="n">
         <v>8</v>
@@ -2921,13 +2921,13 @@
         <v>799157</v>
       </c>
       <c r="O57" s="8" t="n">
-        <v>248581</v>
+        <v>0</v>
       </c>
       <c r="P57" s="8" t="n">
         <v>248581</v>
       </c>
       <c r="Q57" s="8" t="n">
-        <v>0</v>
+        <v>248581</v>
       </c>
       <c r="R57" s="8" t="n">
         <v>0</v>
@@ -2945,19 +2945,19 @@
         </is>
       </c>
       <c r="M58" s="8" t="n">
+        <v>1336084</v>
+      </c>
+      <c r="N58" s="8" t="n">
         <v>1213179</v>
       </c>
-      <c r="N58" s="8" t="n">
-        <v>1336084</v>
-      </c>
       <c r="O58" s="8" t="n">
-        <v>472302</v>
+        <v>122905</v>
       </c>
       <c r="P58" s="8" t="n">
         <v>493356</v>
       </c>
       <c r="Q58" s="8" t="n">
-        <v>122905</v>
+        <v>472302</v>
       </c>
       <c r="R58" s="8" t="n">
         <v>21054</v>
@@ -2995,19 +2995,19 @@
         </is>
       </c>
       <c r="M59" s="8" t="n">
+        <v>1525590</v>
+      </c>
+      <c r="N59" s="8" t="n">
         <v>1519756</v>
       </c>
-      <c r="N59" s="8" t="n">
-        <v>1525590</v>
-      </c>
       <c r="O59" s="8" t="n">
-        <v>1746265</v>
+        <v>5834</v>
       </c>
       <c r="P59" s="8" t="n">
         <v>1744745</v>
       </c>
       <c r="Q59" s="8" t="n">
-        <v>5834</v>
+        <v>1746265</v>
       </c>
       <c r="R59" s="9" t="n">
         <v>-1520</v>
@@ -3037,19 +3037,19 @@
         </is>
       </c>
       <c r="M60" s="8" t="n">
+        <v>6835250</v>
+      </c>
+      <c r="N60" s="8" t="n">
         <v>6328005</v>
       </c>
-      <c r="N60" s="8" t="n">
-        <v>6835250</v>
-      </c>
       <c r="O60" s="8" t="n">
-        <v>3576864</v>
+        <v>507245</v>
       </c>
       <c r="P60" s="8" t="n">
         <v>3700550</v>
       </c>
       <c r="Q60" s="8" t="n">
-        <v>507245</v>
+        <v>3576864</v>
       </c>
       <c r="R60" s="8" t="n">
         <v>123686</v>
@@ -5397,27 +5397,27 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
-          <t>Yesterday Qty. (Mar)</t>
+          <t>02-Feb (Mar)</t>
         </is>
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>Today Qty. (Mar)</t>
+          <t>01-Feb (Mar)</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
-          <t>Yesterday Qty. (Apr)</t>
+          <t>Change (Mar)</t>
         </is>
       </c>
       <c r="E1" s="4" t="inlineStr">
         <is>
-          <t>Today Qty. (Apr)</t>
+          <t>02-Feb (Apr)</t>
         </is>
       </c>
       <c r="F1" s="4" t="inlineStr">
         <is>
-          <t>Change (Mar)</t>
+          <t>01-Feb (Apr)</t>
         </is>
       </c>
       <c r="G1" s="4" t="inlineStr">
@@ -5433,19 +5433,19 @@
         </is>
       </c>
       <c r="B2" s="8" t="n">
+        <v>1219155</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>850580</v>
       </c>
-      <c r="C2" s="8" t="n">
-        <v>1219155</v>
-      </c>
       <c r="D2" s="8" t="n">
-        <v>143975</v>
+        <v>368575</v>
       </c>
       <c r="E2" s="8" t="n">
         <v>248119</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>368575</v>
+        <v>143975</v>
       </c>
       <c r="G2" s="8" t="n">
         <v>104144</v>
@@ -5458,19 +5458,19 @@
         </is>
       </c>
       <c r="B3" s="8" t="n">
+        <v>833429</v>
+      </c>
+      <c r="C3" s="8" t="n">
         <v>832571</v>
       </c>
-      <c r="C3" s="8" t="n">
-        <v>833429</v>
-      </c>
       <c r="D3" s="8" t="n">
-        <v>6462</v>
+        <v>858</v>
       </c>
       <c r="E3" s="8" t="n">
         <v>6462</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>858</v>
+        <v>6462</v>
       </c>
       <c r="G3" s="8" t="n">
         <v>0</v>
@@ -5483,19 +5483,19 @@
         </is>
       </c>
       <c r="B4" s="8" t="n">
+        <v>998102</v>
+      </c>
+      <c r="C4" s="8" t="n">
         <v>989030</v>
       </c>
-      <c r="C4" s="8" t="n">
-        <v>998102</v>
-      </c>
       <c r="D4" s="8" t="n">
-        <v>959279</v>
+        <v>9072</v>
       </c>
       <c r="E4" s="8" t="n">
         <v>959287</v>
       </c>
       <c r="F4" s="8" t="n">
-        <v>9072</v>
+        <v>959279</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>8</v>
@@ -5514,13 +5514,13 @@
         <v>799157</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>248581</v>
+        <v>0</v>
       </c>
       <c r="E5" s="8" t="n">
         <v>248581</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>0</v>
+        <v>248581</v>
       </c>
       <c r="G5" s="8" t="n">
         <v>0</v>
@@ -5533,19 +5533,19 @@
         </is>
       </c>
       <c r="B6" s="8" t="n">
+        <v>1336084</v>
+      </c>
+      <c r="C6" s="8" t="n">
         <v>1213179</v>
       </c>
-      <c r="C6" s="8" t="n">
-        <v>1336084</v>
-      </c>
       <c r="D6" s="8" t="n">
-        <v>472302</v>
+        <v>122905</v>
       </c>
       <c r="E6" s="8" t="n">
         <v>493356</v>
       </c>
       <c r="F6" s="8" t="n">
-        <v>122905</v>
+        <v>472302</v>
       </c>
       <c r="G6" s="8" t="n">
         <v>21054</v>
@@ -5558,19 +5558,19 @@
         </is>
       </c>
       <c r="B7" s="8" t="n">
+        <v>1525590</v>
+      </c>
+      <c r="C7" s="8" t="n">
         <v>1519756</v>
       </c>
-      <c r="C7" s="8" t="n">
-        <v>1525590</v>
-      </c>
       <c r="D7" s="8" t="n">
-        <v>1746265</v>
+        <v>5834</v>
       </c>
       <c r="E7" s="8" t="n">
         <v>1744745</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>5834</v>
+        <v>1746265</v>
       </c>
       <c r="G7" s="9" t="n">
         <v>-1520</v>
@@ -5583,19 +5583,19 @@
         </is>
       </c>
       <c r="B8" s="8" t="n">
+        <v>6835250</v>
+      </c>
+      <c r="C8" s="8" t="n">
         <v>6328005</v>
       </c>
-      <c r="C8" s="8" t="n">
-        <v>6835250</v>
-      </c>
       <c r="D8" s="8" t="n">
-        <v>3576864</v>
+        <v>507245</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>3700550</v>
       </c>
       <c r="F8" s="8" t="n">
-        <v>507245</v>
+        <v>3576864</v>
       </c>
       <c r="G8" s="8" t="n">
         <v>123686</v>

</xml_diff>